<commit_message>
Shared ESS. Input data updated with cost scenarios.
</commit_message>
<xml_diff>
--- a/data/CS3/Shared ESS/CS3_ESS.xlsx
+++ b/data/CS3/Shared ESS/CS3_ESS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS3\Shared ESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459D253-808A-40E2-92A9-BAC08097F6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E44C27-CF7D-41BD-A778-FC6B4D614AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,13 +498,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E1" s="1">
         <v>0.1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E1" s="1">
-        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -1552,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2823AF14-4748-4019-BD7D-F91F970D3C5E}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2075,7 +2075,7 @@
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G1" sqref="G1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Shared ESS. Model updated with cost scenarios.
</commit_message>
<xml_diff>
--- a/data/CS3/Shared ESS/CS3_ESS.xlsx
+++ b/data/CS3/Shared ESS/CS3_ESS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\CS3\Shared ESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E44C27-CF7D-41BD-A778-FC6B4D614AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C609495-7C94-4D5E-8915-A1AA8BD82212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="81" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Investment Cost NREL, USD" sheetId="4" r:id="rId4"/>
     <sheet name="Investment Cost NREL, EUR" sheetId="84" r:id="rId5"/>
     <sheet name="Investment Cost, Power" sheetId="5" r:id="rId6"/>
-    <sheet name="Investment Cost, Capacity" sheetId="85" r:id="rId7"/>
+    <sheet name="Investment Cost, Energy" sheetId="85" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E7A88E-2477-46FD-BE5E-2BB647C1CD4A}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2074,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75013386-D65F-4F42-82AA-9369535BE7EB}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>